<commit_message>
alterando estrutura da tabela e retirando excessos
</commit_message>
<xml_diff>
--- a/banco_dasa.xlsx
+++ b/banco_dasa.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>Funcionario</t>
   </si>
@@ -28,32 +28,50 @@
     <t>Setor</t>
   </si>
   <si>
-    <t>Log</t>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
   <si>
     <t>jorginho</t>
   </si>
   <si>
+    <t>seringa</t>
+  </si>
+  <si>
+    <t>enfermagem</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>15/09/2025</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>seringa</t>
-  </si>
-  <si>
-    <t>enfermagem</t>
-  </si>
-  <si>
-    <t>15/09/2025</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>algodão</t>
+  </si>
+  <si>
+    <t>gazes</t>
+  </si>
+  <si>
+    <t>luvas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,10 +82,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -88,35 +111,70 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -125,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -166,69 +224,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -252,54 +312,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -309,7 +368,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -318,7 +377,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -327,7 +386,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -335,10 +394,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -367,7 +426,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -380,13 +439,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -404,62 +462,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
-        <v>45658</v>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustando filtro de datas
</commit_message>
<xml_diff>
--- a/banco_dasa.xlsx
+++ b/banco_dasa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="45">
   <si>
     <t>Funcionario</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>11:16:01</t>
+  </si>
+  <si>
+    <t>11:24:43</t>
   </si>
   <si>
     <t>15/09/2025</t>
@@ -507,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2037,8 +2040,8 @@
       <c r="E77" t="s">
         <v>42</v>
       </c>
-      <c r="F77" t="s">
-        <v>43</v>
+      <c r="F77" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2057,8 +2060,8 @@
       <c r="E78" t="s">
         <v>42</v>
       </c>
-      <c r="F78" t="s">
-        <v>43</v>
+      <c r="F78" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2077,8 +2080,8 @@
       <c r="E79" t="s">
         <v>42</v>
       </c>
-      <c r="F79" t="s">
-        <v>43</v>
+      <c r="F79" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2097,8 +2100,88 @@
       <c r="E80" t="s">
         <v>42</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
         <v>43</v>
+      </c>
+      <c r="F81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>333</v>
+      </c>
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" t="s">
+        <v>43</v>
+      </c>
+      <c r="F82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>44</v>
+      </c>
+      <c r="D83" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" t="s">
+        <v>43</v>
+      </c>
+      <c r="F83" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>55</v>
+      </c>
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" t="s">
+        <v>43</v>
+      </c>
+      <c r="F84" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando alteracoes perdidas pelo merge
</commit_message>
<xml_diff>
--- a/banco_dasa.xlsx
+++ b/banco_dasa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="48">
   <si>
     <t>Funcionario</t>
   </si>
@@ -64,6 +64,9 @@
     <t>Consultórios</t>
   </si>
   <si>
+    <t>Farmácia</t>
+  </si>
+  <si>
     <t>10:00:00</t>
   </si>
   <si>
@@ -146,6 +149,12 @@
   </si>
   <si>
     <t>11:24:43</t>
+  </si>
+  <si>
+    <t>11:30:08</t>
+  </si>
+  <si>
+    <t>11:31:33</t>
   </si>
   <si>
     <t>15/09/2025</t>
@@ -510,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -550,7 +559,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>45910</v>
@@ -570,7 +579,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
         <v>45911</v>
@@ -587,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2">
         <v>45912</v>
@@ -604,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2">
         <v>45913</v>
@@ -621,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2">
         <v>45915</v>
@@ -638,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <v>45915</v>
@@ -658,7 +667,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2">
         <v>45915</v>
@@ -678,7 +687,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2">
         <v>45915</v>
@@ -698,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2">
         <v>45915</v>
@@ -718,7 +727,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2">
         <v>45915</v>
@@ -738,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2">
         <v>45915</v>
@@ -758,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2">
         <v>45915</v>
@@ -778,7 +787,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2">
         <v>45915</v>
@@ -798,7 +807,7 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2">
         <v>45915</v>
@@ -818,7 +827,7 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2">
         <v>45915</v>
@@ -838,7 +847,7 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2">
         <v>45915</v>
@@ -858,7 +867,7 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18" s="2">
         <v>45915</v>
@@ -878,7 +887,7 @@
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2">
         <v>45915</v>
@@ -898,7 +907,7 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F20" s="2">
         <v>45915</v>
@@ -918,7 +927,7 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F21" s="2">
         <v>45915</v>
@@ -938,7 +947,7 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F22" s="2">
         <v>45915</v>
@@ -958,7 +967,7 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F23" s="2">
         <v>45915</v>
@@ -978,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F24" s="2">
         <v>45915</v>
@@ -998,7 +1007,7 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F25" s="2">
         <v>45915</v>
@@ -1018,7 +1027,7 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F26" s="2">
         <v>45915</v>
@@ -1038,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F27" s="2">
         <v>45915</v>
@@ -1058,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F28" s="2">
         <v>45915</v>
@@ -1078,7 +1087,7 @@
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F29" s="2">
         <v>45915</v>
@@ -1098,7 +1107,7 @@
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F30" s="2">
         <v>45915</v>
@@ -1118,7 +1127,7 @@
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F31" s="2">
         <v>45915</v>
@@ -1138,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F32" s="2">
         <v>45915</v>
@@ -1158,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F33" s="2">
         <v>45915</v>
@@ -1178,7 +1187,7 @@
         <v>14</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F34" s="2">
         <v>45915</v>
@@ -1198,7 +1207,7 @@
         <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F35" s="2">
         <v>45915</v>
@@ -1218,7 +1227,7 @@
         <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F36" s="2">
         <v>45915</v>
@@ -1238,7 +1247,7 @@
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F37" s="2">
         <v>45915</v>
@@ -1258,7 +1267,7 @@
         <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F38" s="2">
         <v>45915</v>
@@ -1278,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F39" s="2">
         <v>45915</v>
@@ -1298,7 +1307,7 @@
         <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F40" s="2">
         <v>45915</v>
@@ -1318,7 +1327,7 @@
         <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F41" s="2">
         <v>45915</v>
@@ -1338,7 +1347,7 @@
         <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F42" s="2">
         <v>45915</v>
@@ -1358,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F43" s="2">
         <v>45915</v>
@@ -1378,7 +1387,7 @@
         <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F44" s="2">
         <v>45915</v>
@@ -1398,7 +1407,7 @@
         <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F45" s="2">
         <v>45915</v>
@@ -1418,7 +1427,7 @@
         <v>14</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F46" s="2">
         <v>45915</v>
@@ -1438,7 +1447,7 @@
         <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F47" s="2">
         <v>45915</v>
@@ -1458,7 +1467,7 @@
         <v>14</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F48" s="2">
         <v>45915</v>
@@ -1478,7 +1487,7 @@
         <v>14</v>
       </c>
       <c r="E49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F49" s="2">
         <v>45915</v>
@@ -1498,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F50" s="2">
         <v>45915</v>
@@ -1518,7 +1527,7 @@
         <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F51" s="2">
         <v>45915</v>
@@ -1538,7 +1547,7 @@
         <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F52" s="2">
         <v>45915</v>
@@ -1558,7 +1567,7 @@
         <v>14</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F53" s="2">
         <v>45915</v>
@@ -1578,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="E54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F54" s="2">
         <v>45915</v>
@@ -1598,7 +1607,7 @@
         <v>14</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F55" s="2">
         <v>45915</v>
@@ -1618,7 +1627,7 @@
         <v>14</v>
       </c>
       <c r="E56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F56" s="2">
         <v>45915</v>
@@ -1638,7 +1647,7 @@
         <v>14</v>
       </c>
       <c r="E57" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F57" s="2">
         <v>45915</v>
@@ -1658,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="E58" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F58" s="2">
         <v>45915</v>
@@ -1678,7 +1687,7 @@
         <v>14</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F59" s="2">
         <v>45915</v>
@@ -1698,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="E60" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F60" s="2">
         <v>45915</v>
@@ -1718,7 +1727,7 @@
         <v>14</v>
       </c>
       <c r="E61" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F61" s="2">
         <v>45915</v>
@@ -1738,7 +1747,7 @@
         <v>14</v>
       </c>
       <c r="E62" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F62" s="2">
         <v>45915</v>
@@ -1758,7 +1767,7 @@
         <v>14</v>
       </c>
       <c r="E63" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F63" s="2">
         <v>45915</v>
@@ -1778,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="E64" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F64" s="2">
         <v>45915</v>
@@ -1798,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="E65" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F65" s="2">
         <v>45915</v>
@@ -1818,7 +1827,7 @@
         <v>14</v>
       </c>
       <c r="E66" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F66" s="2">
         <v>45915</v>
@@ -1838,7 +1847,7 @@
         <v>14</v>
       </c>
       <c r="E67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F67" s="2">
         <v>45915</v>
@@ -1858,7 +1867,7 @@
         <v>14</v>
       </c>
       <c r="E68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F68" s="2">
         <v>45915</v>
@@ -1878,7 +1887,7 @@
         <v>13</v>
       </c>
       <c r="E69" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F69" s="2">
         <v>45915</v>
@@ -1898,7 +1907,7 @@
         <v>13</v>
       </c>
       <c r="E70" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F70" s="2">
         <v>45915</v>
@@ -1918,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F71" s="2">
         <v>45915</v>
@@ -1938,7 +1947,7 @@
         <v>13</v>
       </c>
       <c r="E72" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F72" s="2">
         <v>45915</v>
@@ -1958,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="E73" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F73" s="2">
         <v>45915</v>
@@ -1978,7 +1987,7 @@
         <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F74" s="2">
         <v>45915</v>
@@ -1998,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="E75" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F75" s="2">
         <v>45915</v>
@@ -2018,7 +2027,7 @@
         <v>13</v>
       </c>
       <c r="E76" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F76" s="2">
         <v>45915</v>
@@ -2038,7 +2047,7 @@
         <v>15</v>
       </c>
       <c r="E77" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F77" s="2">
         <v>45915</v>
@@ -2058,7 +2067,7 @@
         <v>15</v>
       </c>
       <c r="E78" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F78" s="2">
         <v>45915</v>
@@ -2078,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="E79" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F79" s="2">
         <v>45915</v>
@@ -2098,7 +2107,7 @@
         <v>15</v>
       </c>
       <c r="E80" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F80" s="2">
         <v>45915</v>
@@ -2118,10 +2127,10 @@
         <v>15</v>
       </c>
       <c r="E81" t="s">
-        <v>43</v>
-      </c>
-      <c r="F81" t="s">
         <v>44</v>
+      </c>
+      <c r="F81" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2138,10 +2147,10 @@
         <v>15</v>
       </c>
       <c r="E82" t="s">
-        <v>43</v>
-      </c>
-      <c r="F82" t="s">
         <v>44</v>
+      </c>
+      <c r="F82" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2158,10 +2167,10 @@
         <v>15</v>
       </c>
       <c r="E83" t="s">
-        <v>43</v>
-      </c>
-      <c r="F83" t="s">
         <v>44</v>
+      </c>
+      <c r="F83" s="2">
+        <v>45915</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2178,10 +2187,170 @@
         <v>15</v>
       </c>
       <c r="E84" t="s">
-        <v>43</v>
-      </c>
-      <c r="F84" t="s">
         <v>44</v>
+      </c>
+      <c r="F84" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86">
+        <v>333</v>
+      </c>
+      <c r="D86" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>44</v>
+      </c>
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88">
+        <v>55</v>
+      </c>
+      <c r="D88" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90">
+        <v>333</v>
+      </c>
+      <c r="D90" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90" t="s">
+        <v>46</v>
+      </c>
+      <c r="F90" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>44</v>
+      </c>
+      <c r="D91" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91" t="s">
+        <v>46</v>
+      </c>
+      <c r="F91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>55</v>
+      </c>
+      <c r="D92" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando menu de confirmacao junto ao copilot
</commit_message>
<xml_diff>
--- a/banco_dasa.xlsx
+++ b/banco_dasa.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labsfiap\Desktop\site-dasa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62931FE5-DCFB-40FC-A11B-065B5E97D3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="51">
   <si>
     <t>Funcionario</t>
   </si>
@@ -61,18 +55,24 @@
     <t>enfermagem</t>
   </si>
   <si>
+    <t>UTI</t>
+  </si>
+  <si>
     <t>Enfermagem</t>
   </si>
   <si>
-    <t>UTI</t>
-  </si>
-  <si>
     <t>Consultórios</t>
   </si>
   <si>
     <t>Farmácia</t>
   </si>
   <si>
+    <t>Limpeza</t>
+  </si>
+  <si>
+    <t>Centro Cirúrgico</t>
+  </si>
+  <si>
     <t>10:00:00</t>
   </si>
   <si>
@@ -136,17 +136,47 @@
     <t>11:31:54</t>
   </si>
   <si>
-    <t>15/09/2025</t>
+    <t>08:59:19</t>
+  </si>
+  <si>
+    <t>09:18:19</t>
+  </si>
+  <si>
+    <t>09:18:42</t>
+  </si>
+  <si>
+    <t>09:21:35</t>
+  </si>
+  <si>
+    <t>09:22:14</t>
+  </si>
+  <si>
+    <t>09:26:59</t>
+  </si>
+  <si>
+    <t>09:35:29</t>
+  </si>
+  <si>
+    <t>09:35:54</t>
+  </si>
+  <si>
+    <t>09:37:56</t>
+  </si>
+  <si>
+    <t>09:38:16</t>
+  </si>
+  <si>
+    <t>19/09/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,14 +240,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,27 +318,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,24 +352,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -541,24 +527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -592,13 +568,13 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2">
         <v>45910</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -609,16 +585,16 @@
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -629,16 +605,16 @@
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -649,16 +625,16 @@
         <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -669,16 +645,16 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -689,16 +665,16 @@
         <v>300</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -709,16 +685,16 @@
         <v>300</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -729,16 +705,16 @@
         <v>300</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -749,16 +725,16 @@
         <v>300</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -769,16 +745,16 @@
         <v>300</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -789,16 +765,16 @@
         <v>300</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F12" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -809,16 +785,16 @@
         <v>300</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -829,16 +805,16 @@
         <v>450</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F14" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -849,16 +825,16 @@
         <v>450</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -869,16 +845,16 @@
         <v>450</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F16" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -889,16 +865,16 @@
         <v>450</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -909,16 +885,16 @@
         <v>450</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F18" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -929,16 +905,16 @@
         <v>450</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F19" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -949,16 +925,16 @@
         <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -969,16 +945,16 @@
         <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F21" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -989,16 +965,16 @@
         <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1009,16 +985,16 @@
         <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F23" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1029,16 +1005,16 @@
         <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F24" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1049,16 +1025,16 @@
         <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F25" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1069,16 +1045,16 @@
         <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F26" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1089,16 +1065,16 @@
         <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F27" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1109,16 +1085,16 @@
         <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F28" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1129,16 +1105,16 @@
         <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F29" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1149,16 +1125,16 @@
         <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F30" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1169,16 +1145,16 @@
         <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F31" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1189,16 +1165,16 @@
         <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F32" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1209,16 +1185,16 @@
         <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1229,16 +1205,16 @@
         <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F34" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1249,16 +1225,16 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F35" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1269,16 +1245,16 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F36" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1289,16 +1265,16 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F37" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1312,13 +1288,13 @@
         <v>15</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F38" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1332,13 +1308,13 @@
         <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F39" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1352,13 +1328,13 @@
         <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F40" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1372,13 +1348,13 @@
         <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F41" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1392,13 +1368,13 @@
         <v>15</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F42" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1412,13 +1388,13 @@
         <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F43" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1432,13 +1408,13 @@
         <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F44" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1452,13 +1428,13 @@
         <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F45" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1472,13 +1448,13 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F46" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1492,13 +1468,13 @@
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F47" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1512,13 +1488,13 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F48" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1532,13 +1508,13 @@
         <v>16</v>
       </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F49" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1552,13 +1528,13 @@
         <v>16</v>
       </c>
       <c r="E50" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F50" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1572,13 +1548,13 @@
         <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F51" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1592,13 +1568,13 @@
         <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F52" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1612,13 +1588,13 @@
         <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F53" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1632,13 +1608,13 @@
         <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F54" s="2">
         <v>45915</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1652,10 +1628,510 @@
         <v>16</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
-      </c>
-      <c r="F55" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="F55" s="2">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" t="s">
+        <v>47</v>
+      </c>
+      <c r="F72" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" t="s">
+        <v>47</v>
+      </c>
+      <c r="F73" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" t="s">
+        <v>47</v>
+      </c>
+      <c r="F74" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" t="s">
+        <v>48</v>
+      </c>
+      <c r="F77" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando readme e testando site
</commit_message>
<xml_diff>
--- a/banco_dasa.xlsx
+++ b/banco_dasa.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labsfiap\Desktop\site-dasa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818E8145-CBD0-4D35-8E83-4C7DC3FFB09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="54">
   <si>
     <t>Funcionario</t>
   </si>
@@ -166,29 +160,32 @@
     <t>09:35:54</t>
   </si>
   <si>
+    <t>09:38:16</t>
+  </si>
+  <si>
     <t>09:37:56</t>
   </si>
   <si>
-    <t>09:38:16</t>
-  </si>
-  <si>
     <t>10:29:19</t>
   </si>
   <si>
     <t>10:29:56</t>
   </si>
   <si>
-    <t>19/09/2025</t>
+    <t>14:29:24</t>
+  </si>
+  <si>
+    <t>20/09/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,14 +249,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -306,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -338,27 +327,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,24 +361,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -583,19 +536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -635,7 +583,7 @@
         <v>45910</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -655,7 +603,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -675,7 +623,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -695,7 +643,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -715,7 +663,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -735,7 +683,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -755,7 +703,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -775,7 +723,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -795,7 +743,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -815,7 +763,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -835,7 +783,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -855,7 +803,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -875,7 +823,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -895,7 +843,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -915,7 +863,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -935,7 +883,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -955,7 +903,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -975,7 +923,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -995,7 +943,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +963,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1035,7 +983,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1003,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1023,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1043,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1063,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1083,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1155,7 +1103,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1123,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1143,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1163,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1183,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1255,7 +1203,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1275,7 +1223,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1295,7 +1243,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1315,7 +1263,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1335,7 +1283,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1355,7 +1303,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1323,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1395,7 +1343,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1363,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1383,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +1403,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1423,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1443,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1463,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1483,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1555,7 +1503,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1575,7 +1523,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1595,7 +1543,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1563,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1583,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1655,7 +1603,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1675,7 +1623,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1643,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1715,7 +1663,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1735,7 +1683,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -1755,7 +1703,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1723,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1795,7 +1743,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1763,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -1835,7 +1783,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -1855,7 +1803,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +1823,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1843,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -1915,7 +1863,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -1935,7 +1883,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1955,7 +1903,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +1923,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -1995,7 +1943,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -2015,7 +1963,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -2035,7 +1983,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -2055,7 +2003,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -2075,7 +2023,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -2095,7 +2043,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2063,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -2135,7 +2083,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -2149,13 +2097,13 @@
         <v>13</v>
       </c>
       <c r="E78" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F78" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -2169,13 +2117,13 @@
         <v>13</v>
       </c>
       <c r="E79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F79" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -2189,13 +2137,13 @@
         <v>13</v>
       </c>
       <c r="E80" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F80" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -2209,13 +2157,13 @@
         <v>18</v>
       </c>
       <c r="E81" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F81" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -2229,13 +2177,13 @@
         <v>18</v>
       </c>
       <c r="E82" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F82" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -2249,13 +2197,13 @@
         <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F83" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -2269,13 +2217,13 @@
         <v>13</v>
       </c>
       <c r="E84" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F84" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -2289,13 +2237,13 @@
         <v>13</v>
       </c>
       <c r="E85" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F85" s="2">
         <v>45919</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -2315,7 +2263,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -2335,7 +2283,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -2355,7 +2303,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -2375,7 +2323,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -2391,11 +2339,11 @@
       <c r="E90" t="s">
         <v>51</v>
       </c>
-      <c r="F90" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -2411,11 +2359,11 @@
       <c r="E91" t="s">
         <v>51</v>
       </c>
-      <c r="F91" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -2431,11 +2379,11 @@
       <c r="E92" t="s">
         <v>51</v>
       </c>
-      <c r="F92" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -2451,8 +2399,68 @@
       <c r="E93" t="s">
         <v>51</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="2">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>123</v>
+      </c>
+      <c r="D94" t="s">
+        <v>14</v>
+      </c>
+      <c r="E94" t="s">
         <v>52</v>
+      </c>
+      <c r="F94" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" t="s">
+        <v>52</v>
+      </c>
+      <c r="F95" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>3</v>
+      </c>
+      <c r="D96" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>52</v>
+      </c>
+      <c r="F96" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>